<commit_message>
refactor and add more data
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -388,10 +388,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.05703064225662539</v>
+        <v>0.01652577235857634</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06925364760893234</v>
+        <v>0.03347919488030672</v>
       </c>
     </row>
     <row r="3">
@@ -399,10 +399,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04665375004962953</v>
+        <v>0.01927675928009841</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05532619331593329</v>
+        <v>0.03636165096783885</v>
       </c>
     </row>
     <row r="4">
@@ -410,10 +410,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0332879091915035</v>
+        <v>0.02159953269702994</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04118038378194754</v>
+        <v>0.04077332017719157</v>
       </c>
     </row>
     <row r="5">
@@ -421,10 +421,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0339095295020149</v>
+        <v>0.02285051840486269</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04173801944623075</v>
+        <v>0.04349266310446182</v>
       </c>
     </row>
     <row r="6">
@@ -432,10 +432,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.03204785725073482</v>
+        <v>0.02520421430104667</v>
       </c>
       <c r="C6" t="n">
-        <v>0.04264579953962784</v>
+        <v>0.04831450552228939</v>
       </c>
     </row>
     <row r="7">
@@ -443,10 +443,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.03160259949606917</v>
+        <v>0.02294172383415028</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04161362697235838</v>
+        <v>0.04624239128749408</v>
       </c>
     </row>
     <row r="8">
@@ -454,10 +454,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02987715960033617</v>
+        <v>0.02421330825042563</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03645286897858217</v>
+        <v>0.0483049256956185</v>
       </c>
     </row>
     <row r="9">
@@ -465,10 +465,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.02787804469072297</v>
+        <v>0.02588327534669511</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03260288652610758</v>
+        <v>0.04839857970646459</v>
       </c>
     </row>
     <row r="10">
@@ -476,10 +476,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02735504224441466</v>
+        <v>0.02660737802725797</v>
       </c>
       <c r="C10" t="n">
-        <v>0.03318479588232053</v>
+        <v>0.05635550058836643</v>
       </c>
     </row>
     <row r="11">
@@ -487,10 +487,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.02689368732733398</v>
+        <v>0.02819156066213258</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03461341441718414</v>
+        <v>0.0575588030636747</v>
       </c>
     </row>
     <row r="12">
@@ -498,10 +498,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0233825601085968</v>
+        <v>0.02833601731714437</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03013436583979228</v>
+        <v>0.05688414398712061</v>
       </c>
     </row>
     <row r="13">
@@ -509,10 +509,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>0.02324656082211966</v>
+        <v>0.02656732681116657</v>
       </c>
       <c r="C13" t="n">
-        <v>0.03132570975862575</v>
+        <v>0.0507410754640036</v>
       </c>
     </row>
     <row r="14">
@@ -520,10 +520,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02278034615690026</v>
+        <v>0.02849029058414042</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03117025600221405</v>
+        <v>0.05428956764375461</v>
       </c>
     </row>
     <row r="15">
@@ -531,10 +531,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>0.02165104695905977</v>
+        <v>0.02768074674960684</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03019105909212479</v>
+        <v>0.05029263491849386</v>
       </c>
     </row>
     <row r="16">
@@ -542,10 +542,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0218031988503503</v>
+        <v>0.02803702131581991</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03195060217504173</v>
+        <v>0.05413640313146839</v>
       </c>
     </row>
     <row r="17">
@@ -553,10 +553,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02176709800112223</v>
+        <v>0.02877949356325445</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02993857098637911</v>
+        <v>0.05222792004919209</v>
       </c>
     </row>
     <row r="18">
@@ -564,10 +564,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>0.02061123002806322</v>
+        <v>0.02832971697418312</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02629787267165377</v>
+        <v>0.05245502903561287</v>
       </c>
     </row>
     <row r="19">
@@ -575,10 +575,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>0.02065093903214617</v>
+        <v>0.02746171320502883</v>
       </c>
       <c r="C19" t="n">
-        <v>0.02613554552101793</v>
+        <v>0.05117971212170454</v>
       </c>
     </row>
     <row r="20">
@@ -586,10 +586,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>0.01947905620648133</v>
+        <v>0.02807359794915116</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02570408473181189</v>
+        <v>0.05398631178995315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>